<commit_message>
flutter connected with logic
</commit_message>
<xml_diff>
--- a/database/questions.xlsx
+++ b/database/questions.xlsx
@@ -146,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -165,6 +165,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,7 +452,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,7 +497,7 @@
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1">
@@ -520,7 +523,7 @@
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1">
@@ -546,7 +549,7 @@
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1">
@@ -572,7 +575,7 @@
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1">

</xml_diff>